<commit_message>
Actualización Propuesta Económica V3
</commit_message>
<xml_diff>
--- a/Ventas/Propuesta Económica/Propuesta Económica V3.xlsx
+++ b/Ventas/Propuesta Económica/Propuesta Económica V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\AntirShadow\Downloads\WebGL\ProyectoRedes\Ventas\Propuesta Económica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D9C3B3-E2C7-4568-B181-74AA96950185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AF1B30-7938-4B18-894B-8E0D03671B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>$1 US</t>
   </si>
   <si>
-    <t>$ 18.05 MXN</t>
-  </si>
-  <si>
     <t>VIGENCIA</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>https://www.tradeinn.com/techinn/es/cisco-isr4321-sec/137369272/p?queryID=535d7781121dee72e81a9ffbef39510a&amp;buscador_search</t>
+  </si>
+  <si>
+    <t>$ 18.01 MXN</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -173,10 +173,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -197,12 +193,6 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -231,6 +221,14 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -256,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -269,68 +267,41 @@
         <color rgb="FF3F3F3F"/>
       </left>
       <right/>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -551,10 +522,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -568,18 +539,20 @@
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" ht="36.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -593,7 +566,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -605,198 +578,195 @@
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10">
         <v>5159</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10">
+      <c r="E3" s="10"/>
+      <c r="F3" s="9">
         <f t="shared" ref="F3:F4" si="0">D3*C3</f>
         <v>0</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="12" t="s">
-        <v>17</v>
+      <c r="G3" s="8"/>
+      <c r="H3" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="10">
         <v>8159</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="10">
+      <c r="E4" s="10"/>
+      <c r="F4" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="12" t="s">
-        <v>18</v>
+      <c r="G4" s="8"/>
+      <c r="H4" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>8639</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="10">
+      <c r="E5" s="7"/>
+      <c r="F5" s="9">
         <f>D5*C5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="12" t="s">
-        <v>19</v>
+      <c r="G5" s="8"/>
+      <c r="H5" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>24</v>
+      <c r="B6" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>8969</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="10">
+      <c r="E6" s="7"/>
+      <c r="F6" s="9">
         <f t="shared" ref="F6:F10" si="1">D6*C6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="12" t="s">
-        <v>20</v>
+      <c r="G6" s="8"/>
+      <c r="H6" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>12549</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>9064.99</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>30</v>
+      <c r="G7" s="8"/>
+      <c r="H7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>13169</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="10">
+      <c r="E8" s="7"/>
+      <c r="F8" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>22</v>
+      <c r="H8" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>27</v>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>22239</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="10">
+      <c r="E9" s="7"/>
+      <c r="F9" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>23</v>
+      <c r="H9" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>36</v>
+      <c r="B10" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>11310</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>29</v>
+      <c r="H10" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>37</v>
+      <c r="B11" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>40718.99</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="2"/>
       <c r="H11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -804,125 +774,55 @@
       <c r="F12" s="2"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="7:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="7:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="7:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    </row>
+    <row r="25" spans="7:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G25" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G28" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G30" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G31" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{9E54A654-BD10-441A-9474-B1574C495146}"/>
@@ -933,9 +833,9 @@
     <hyperlink ref="H8" r:id="rId6" xr:uid="{632F6377-213C-4148-90C8-70FA7B855FDA}"/>
     <hyperlink ref="H9" r:id="rId7" xr:uid="{62E4BDBB-DD05-43BC-9221-D706E7BAF10D}"/>
     <hyperlink ref="I7" r:id="rId8" xr:uid="{D20C444D-136A-4695-84CD-A33EDE128237}"/>
-    <hyperlink ref="C22" r:id="rId9" xr:uid="{62E13CD6-7C24-4625-8070-CEFD3BC5D67F}"/>
+    <hyperlink ref="C16" r:id="rId9" xr:uid="{62E13CD6-7C24-4625-8070-CEFD3BC5D67F}"/>
     <hyperlink ref="H10" r:id="rId10" xr:uid="{B1A962DA-5618-4391-8E78-D821E44FCADE}"/>
-    <hyperlink ref="C20" r:id="rId11" xr:uid="{0880B30E-8CE6-4492-AF3E-A144FAA66348}"/>
+    <hyperlink ref="C14" r:id="rId11" xr:uid="{0880B30E-8CE6-4492-AF3E-A144FAA66348}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>

</xml_diff>